<commit_message>
updating sheets to conform to standard
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_1045.xlsx
+++ b/bioSample/bioSample_1045.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/old_database/crypto/bioSample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849DDBB3-C187-7D4C-BC16-82B20C748148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0B4290-D302-6344-9185-B82068C8D018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="23">
   <si>
     <t>harvestDate</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>90minuteInduction</t>
+  </si>
+  <si>
+    <t>TDY1480</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D19"/>
+      <selection activeCell="F17" sqref="F17:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -720,6 +723,9 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
       <c r="G8" t="s">
         <v>15</v>
       </c>
@@ -746,6 +752,9 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" t="s">
         <v>15</v>
       </c>
@@ -772,6 +781,9 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
       <c r="G10" t="s">
         <v>15</v>
       </c>
@@ -972,6 +984,9 @@
       <c r="D17" t="s">
         <v>21</v>
       </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
       <c r="G17" t="s">
         <v>15</v>
       </c>
@@ -998,6 +1013,9 @@
       <c r="D18" t="s">
         <v>21</v>
       </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
       <c r="G18" t="s">
         <v>15</v>
       </c>
@@ -1023,6 +1041,9 @@
       </c>
       <c r="D19" t="s">
         <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
       </c>
       <c r="G19" t="s">
         <v>15</v>

</xml_diff>